<commit_message>
prehladavanie do sirky, hlbky upravy
prehladavanie do sirky, hlbky upravy
</commit_message>
<xml_diff>
--- a/algoritmy.xlsx
+++ b/algoritmy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\UNIZA\semester 2\teoria grafov\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\ATG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F7A39A-F514-43B7-AC4B-2169CDCEF0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE685FD-9337-4EE0-B2E0-8034D2E76A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="7" xr2:uid="{58D429C4-09FB-489B-BF23-3DBAB713922B}"/>
+    <workbookView xWindow="1320" yWindow="960" windowWidth="17280" windowHeight="9960" firstSheet="6" activeTab="7" xr2:uid="{58D429C4-09FB-489B-BF23-3DBAB713922B}"/>
   </bookViews>
   <sheets>
     <sheet name="Zakladny alg." sheetId="1" r:id="rId1"/>
@@ -1248,6 +1248,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1265,9 +1268,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3817,23 +3817,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="C34:J34"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="L26:M26"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7104,15 +7104,15 @@
       <c r="G5" s="65"/>
       <c r="H5" s="65"/>
       <c r="I5" s="65"/>
-      <c r="J5" s="70" t="s">
+      <c r="J5" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="71"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="15"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="69"/>
-      <c r="B6" s="69"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="4">
         <v>1</v>
       </c>
@@ -7134,8 +7134,8 @@
       <c r="I6" s="4">
         <v>7</v>
       </c>
-      <c r="J6" s="72"/>
-      <c r="K6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="74"/>
       <c r="L6" s="15"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -7162,10 +7162,10 @@
       <c r="I7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="68" t="s">
+      <c r="J7" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="K7" s="68"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="15"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -7182,10 +7182,10 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="68" t="s">
+      <c r="J8" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="68"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="15"/>
       <c r="M8" t="s">
         <v>26</v>
@@ -7226,10 +7226,10 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="68" t="s">
+      <c r="J9" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="K9" s="68"/>
+      <c r="K9" s="69"/>
       <c r="L9" s="15"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -7246,10 +7246,10 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="68" t="s">
+      <c r="J10" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="K10" s="68"/>
+      <c r="K10" s="69"/>
       <c r="L10" s="15"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -7270,10 +7270,10 @@
       <c r="I11" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="J11" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="K11" s="68"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="15" t="s">
         <v>107</v>
       </c>
@@ -7297,10 +7297,10 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="68" t="s">
+      <c r="J12" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="K12" s="68"/>
+      <c r="K12" s="69"/>
       <c r="L12" s="15" t="s">
         <v>113</v>
       </c>
@@ -7319,10 +7319,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="68" t="s">
+      <c r="J13" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="K13" s="68"/>
+      <c r="K13" s="69"/>
       <c r="L13" s="15"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -7341,10 +7341,10 @@
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="68" t="s">
+      <c r="J14" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="K14" s="68"/>
+      <c r="K14" s="69"/>
       <c r="L14" s="15" t="s">
         <v>115</v>
       </c>
@@ -7363,10 +7363,10 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="68">
+      <c r="J15" s="69">
         <v>5</v>
       </c>
-      <c r="K15" s="68"/>
+      <c r="K15" s="69"/>
       <c r="L15" s="15"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
@@ -7385,10 +7385,10 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="68">
-        <v>2</v>
-      </c>
-      <c r="K16" s="68"/>
+      <c r="J16" s="69">
+        <v>2</v>
+      </c>
+      <c r="K16" s="69"/>
       <c r="L16" s="15" t="s">
         <v>117</v>
       </c>
@@ -7409,10 +7409,10 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="74">
-        <v>1</v>
-      </c>
-      <c r="K17" s="74"/>
+      <c r="J17" s="68">
+        <v>1</v>
+      </c>
+      <c r="K17" s="68"/>
       <c r="L17" s="15" t="s">
         <v>118</v>
       </c>
@@ -7433,10 +7433,10 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="74">
-        <v>3</v>
-      </c>
-      <c r="K18" s="74"/>
+      <c r="J18" s="68">
+        <v>3</v>
+      </c>
+      <c r="K18" s="68"/>
       <c r="L18" s="15" t="s">
         <v>121</v>
       </c>
@@ -7457,10 +7457,10 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="74">
-        <v>4</v>
-      </c>
-      <c r="K19" s="74"/>
+      <c r="J19" s="68">
+        <v>4</v>
+      </c>
+      <c r="K19" s="68"/>
       <c r="L19" s="15" t="s">
         <v>123</v>
       </c>
@@ -7470,13 +7470,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J12:K12"/>
@@ -7488,6 +7481,13 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7564,7 +7564,7 @@
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="70" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="53" t="s">
@@ -8066,7 +8066,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8132,7 +8132,7 @@
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="70" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="53" t="s">
@@ -8701,7 +8701,7 @@
       <c r="B5" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="70" t="s">
         <v>168</v>
       </c>
       <c r="D5" s="65" t="s">

</xml_diff>